<commit_message>
Added more wind data
</commit_message>
<xml_diff>
--- a/WindSpeed.xlsx
+++ b/WindSpeed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Louis/Drive/Bristol/Personal/Hackathon/EcoOptimiser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Louis/Documents/Git Repos/EcoOptimiser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Location</t>
   </si>
@@ -135,6 +135,114 @@
   </si>
   <si>
     <t>Norwich</t>
+  </si>
+  <si>
+    <t>Isle Of Man</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Eglinton</t>
+  </si>
+  <si>
+    <t>Valley</t>
+  </si>
+  <si>
+    <t>Pembrey Sands</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Coventry</t>
+  </si>
+  <si>
+    <t>Marham</t>
+  </si>
+  <si>
+    <t>Wattisham</t>
+  </si>
+  <si>
+    <t>Manston</t>
+  </si>
+  <si>
+    <t>Lydd</t>
+  </si>
+  <si>
+    <t>Shoreham</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Newquay</t>
+  </si>
+  <si>
+    <t>Culdrose</t>
+  </si>
+  <si>
+    <t>Scilly</t>
+  </si>
+  <si>
+    <t>Alderney</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Heathrow</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Lyneham</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Filton</t>
+  </si>
+  <si>
+    <t>Yeovilton</t>
+  </si>
+  <si>
+    <t>Bournemouth</t>
+  </si>
+  <si>
+    <t>Gatwick</t>
+  </si>
+  <si>
+    <t>Brize Norton</t>
+  </si>
+  <si>
+    <t>Cheltenham</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Cranfield</t>
+  </si>
+  <si>
+    <t>Luton</t>
+  </si>
+  <si>
+    <t>Stansted</t>
+  </si>
+  <si>
+    <t>Tiree</t>
+  </si>
+  <si>
+    <t>Islay</t>
+  </si>
+  <si>
+    <t>Campbeltown</t>
+  </si>
+  <si>
+    <t>Prestwick</t>
   </si>
 </sst>
 </file>
@@ -179,7 +287,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -473,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +828,7 @@
         <v>5.95</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P26" si="0">AVERAGE(D4:O4)</f>
+        <f t="shared" ref="P4:P55" si="0">AVERAGE(D4:O4)</f>
         <v>5.7341666666666669</v>
       </c>
     </row>
@@ -1519,6 +1697,1834 @@
       <c r="P21">
         <f t="shared" si="0"/>
         <v>4.5966666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>54.083300000000001</v>
+      </c>
+      <c r="C22">
+        <v>-4.6332000000000004</v>
+      </c>
+      <c r="D22">
+        <v>8.16</v>
+      </c>
+      <c r="E22">
+        <v>6.4</v>
+      </c>
+      <c r="F22">
+        <v>6.92</v>
+      </c>
+      <c r="G22">
+        <v>5.68</v>
+      </c>
+      <c r="H22">
+        <v>5.84</v>
+      </c>
+      <c r="I22">
+        <v>4.83</v>
+      </c>
+      <c r="J22">
+        <v>5.26</v>
+      </c>
+      <c r="K22">
+        <v>5.68</v>
+      </c>
+      <c r="L22">
+        <v>5.97</v>
+      </c>
+      <c r="M22">
+        <v>6.84</v>
+      </c>
+      <c r="N22">
+        <v>7.71</v>
+      </c>
+      <c r="O22">
+        <v>7.06</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="0"/>
+        <v>6.3624999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>54.6</v>
+      </c>
+      <c r="C23">
+        <v>-5.8832899999999997</v>
+      </c>
+      <c r="D23">
+        <v>5.46</v>
+      </c>
+      <c r="E23">
+        <v>4.62</v>
+      </c>
+      <c r="F23">
+        <v>5.29</v>
+      </c>
+      <c r="G23">
+        <v>4.97</v>
+      </c>
+      <c r="H23">
+        <v>5.03</v>
+      </c>
+      <c r="I23">
+        <v>4.55</v>
+      </c>
+      <c r="J23">
+        <v>4.58</v>
+      </c>
+      <c r="K23">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="L23">
+        <v>4.57</v>
+      </c>
+      <c r="M23">
+        <v>4.63</v>
+      </c>
+      <c r="N23">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="O23">
+        <v>4.41</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="0"/>
+        <v>4.8008333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>55.05</v>
+      </c>
+      <c r="C24">
+        <v>-7.1499899999999998</v>
+      </c>
+      <c r="D24">
+        <v>5.85</v>
+      </c>
+      <c r="E24">
+        <v>4.68</v>
+      </c>
+      <c r="F24">
+        <v>5.57</v>
+      </c>
+      <c r="G24">
+        <v>5.25</v>
+      </c>
+      <c r="H24">
+        <v>5.38</v>
+      </c>
+      <c r="I24">
+        <v>4.68</v>
+      </c>
+      <c r="J24">
+        <v>4.71</v>
+      </c>
+      <c r="K24">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="L24">
+        <v>4.87</v>
+      </c>
+      <c r="M24">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="N24">
+        <v>5.39</v>
+      </c>
+      <c r="O24">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="0"/>
+        <v>5.0333333333333341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>53.25</v>
+      </c>
+      <c r="C25">
+        <v>-4.5332999999999997</v>
+      </c>
+      <c r="D25">
+        <v>7.8</v>
+      </c>
+      <c r="E25">
+        <v>5.73</v>
+      </c>
+      <c r="F25">
+        <v>6.87</v>
+      </c>
+      <c r="G25">
+        <v>5.69</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="I25">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="J25">
+        <v>5.98</v>
+      </c>
+      <c r="K25">
+        <v>6.2</v>
+      </c>
+      <c r="L25">
+        <v>6.05</v>
+      </c>
+      <c r="M25">
+        <v>6.62</v>
+      </c>
+      <c r="N25">
+        <v>7.48</v>
+      </c>
+      <c r="O25">
+        <v>6.57</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>6.3275000000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26">
+        <v>51.716700000000003</v>
+      </c>
+      <c r="C26">
+        <v>-4.3666999999999998</v>
+      </c>
+      <c r="D26">
+        <v>7.06</v>
+      </c>
+      <c r="E26">
+        <v>5.42</v>
+      </c>
+      <c r="F26">
+        <v>6.62</v>
+      </c>
+      <c r="G26">
+        <v>5.33</v>
+      </c>
+      <c r="H26">
+        <v>5.98</v>
+      </c>
+      <c r="I26">
+        <v>4.91</v>
+      </c>
+      <c r="J26">
+        <v>6.76</v>
+      </c>
+      <c r="K26">
+        <v>6.64</v>
+      </c>
+      <c r="L26">
+        <v>6.06</v>
+      </c>
+      <c r="M26">
+        <v>6.23</v>
+      </c>
+      <c r="N26">
+        <v>7.39</v>
+      </c>
+      <c r="O26">
+        <v>6.11</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>6.2091666666666674</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27">
+        <v>51.4</v>
+      </c>
+      <c r="C27">
+        <v>-3.4333</v>
+      </c>
+      <c r="D27">
+        <v>5.55</v>
+      </c>
+      <c r="E27">
+        <v>4.59</v>
+      </c>
+      <c r="F27">
+        <v>5.4</v>
+      </c>
+      <c r="G27">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>3.98</v>
+      </c>
+      <c r="J27">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="K27">
+        <v>4.53</v>
+      </c>
+      <c r="L27">
+        <v>4.3</v>
+      </c>
+      <c r="M27">
+        <v>4.53</v>
+      </c>
+      <c r="N27">
+        <v>5.42</v>
+      </c>
+      <c r="O27">
+        <v>4.92</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>4.7791666666666677</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>52.366700000000002</v>
+      </c>
+      <c r="C28">
+        <v>-1.4832989999999999</v>
+      </c>
+      <c r="D28">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E28">
+        <v>3.97</v>
+      </c>
+      <c r="F28">
+        <v>4.96</v>
+      </c>
+      <c r="G28">
+        <v>4.12</v>
+      </c>
+      <c r="H28">
+        <v>4.32</v>
+      </c>
+      <c r="I28">
+        <v>3.56</v>
+      </c>
+      <c r="J28">
+        <v>3.93</v>
+      </c>
+      <c r="K28">
+        <v>3.96</v>
+      </c>
+      <c r="L28">
+        <v>3.77</v>
+      </c>
+      <c r="M28">
+        <v>3.61</v>
+      </c>
+      <c r="N28">
+        <v>4.29</v>
+      </c>
+      <c r="O28">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>4.1350000000000007</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>52.65</v>
+      </c>
+      <c r="C29">
+        <v>0.56669000000000003</v>
+      </c>
+      <c r="D29">
+        <v>5.45</v>
+      </c>
+      <c r="E29">
+        <v>4.42</v>
+      </c>
+      <c r="F29">
+        <v>5.44</v>
+      </c>
+      <c r="G29">
+        <v>4.49</v>
+      </c>
+      <c r="H29">
+        <v>4.76</v>
+      </c>
+      <c r="I29">
+        <v>3.91</v>
+      </c>
+      <c r="J29">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="K29">
+        <v>4.59</v>
+      </c>
+      <c r="L29">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="M29">
+        <v>4.42</v>
+      </c>
+      <c r="N29">
+        <v>5.17</v>
+      </c>
+      <c r="O29">
+        <v>4.51</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>4.6658333333333344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>52.116700000000002</v>
+      </c>
+      <c r="C30">
+        <v>0.96669899999999997</v>
+      </c>
+      <c r="D30">
+        <v>5.27</v>
+      </c>
+      <c r="E30">
+        <v>4.62</v>
+      </c>
+      <c r="F30">
+        <v>5.34</v>
+      </c>
+      <c r="G30">
+        <v>4.33</v>
+      </c>
+      <c r="H30">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="I30">
+        <v>3.91</v>
+      </c>
+      <c r="J30">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="K30">
+        <v>4.46</v>
+      </c>
+      <c r="L30">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="M30">
+        <v>4.24</v>
+      </c>
+      <c r="N30">
+        <v>4.99</v>
+      </c>
+      <c r="O30">
+        <v>4.66</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>4.5883333333333338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>51.333300000000001</v>
+      </c>
+      <c r="C31">
+        <v>1.3460989999999999</v>
+      </c>
+      <c r="D31">
+        <v>6.05</v>
+      </c>
+      <c r="E31">
+        <v>5.59</v>
+      </c>
+      <c r="F31">
+        <v>6.01</v>
+      </c>
+      <c r="G31">
+        <v>5.03</v>
+      </c>
+      <c r="H31">
+        <v>5.67</v>
+      </c>
+      <c r="I31">
+        <v>4.78</v>
+      </c>
+      <c r="J31">
+        <v>5.33</v>
+      </c>
+      <c r="K31">
+        <v>5.5</v>
+      </c>
+      <c r="L31">
+        <v>5.39</v>
+      </c>
+      <c r="M31">
+        <v>5.27</v>
+      </c>
+      <c r="N31">
+        <v>6.11</v>
+      </c>
+      <c r="O31">
+        <v>5.56</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>5.5241666666666669</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>50.95</v>
+      </c>
+      <c r="C32">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="D32">
+        <v>6.95</v>
+      </c>
+      <c r="E32">
+        <v>6.17</v>
+      </c>
+      <c r="F32">
+        <v>7.3</v>
+      </c>
+      <c r="G32">
+        <v>6.3</v>
+      </c>
+      <c r="H32">
+        <v>7.02</v>
+      </c>
+      <c r="I32">
+        <v>6.23</v>
+      </c>
+      <c r="J32">
+        <v>7.21</v>
+      </c>
+      <c r="K32">
+        <v>6.93</v>
+      </c>
+      <c r="L32">
+        <v>6.5</v>
+      </c>
+      <c r="M32">
+        <v>6.23</v>
+      </c>
+      <c r="N32">
+        <v>6.9</v>
+      </c>
+      <c r="O32">
+        <v>6.35</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>6.6741666666666672</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>50.832999999999998</v>
+      </c>
+      <c r="C33">
+        <v>-0.2833</v>
+      </c>
+      <c r="D33">
+        <v>5.54</v>
+      </c>
+      <c r="E33">
+        <v>4.84</v>
+      </c>
+      <c r="F33">
+        <v>5.37</v>
+      </c>
+      <c r="G33">
+        <v>4.71</v>
+      </c>
+      <c r="H33">
+        <v>5.39</v>
+      </c>
+      <c r="I33">
+        <v>4.76</v>
+      </c>
+      <c r="J33">
+        <v>5.48</v>
+      </c>
+      <c r="K33">
+        <v>5.39</v>
+      </c>
+      <c r="L33">
+        <v>4.93</v>
+      </c>
+      <c r="M33">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="N33">
+        <v>5.52</v>
+      </c>
+      <c r="O33">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>5.1466666666666674</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34">
+        <v>50.9</v>
+      </c>
+      <c r="C34">
+        <v>-1.3998999999999999</v>
+      </c>
+      <c r="D34">
+        <v>3.68</v>
+      </c>
+      <c r="E34">
+        <v>3.13</v>
+      </c>
+      <c r="F34">
+        <v>3.88</v>
+      </c>
+      <c r="G34">
+        <v>3.3</v>
+      </c>
+      <c r="H34">
+        <v>3.7</v>
+      </c>
+      <c r="I34">
+        <v>3.27</v>
+      </c>
+      <c r="J34">
+        <v>3.87</v>
+      </c>
+      <c r="K34">
+        <v>3.63</v>
+      </c>
+      <c r="L34">
+        <v>3.07</v>
+      </c>
+      <c r="M34">
+        <v>2.79</v>
+      </c>
+      <c r="N34">
+        <v>3.41</v>
+      </c>
+      <c r="O34">
+        <v>2.88</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="0"/>
+        <v>3.3841666666666672</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35">
+        <v>50.433300000000003</v>
+      </c>
+      <c r="C35">
+        <v>-5</v>
+      </c>
+      <c r="D35">
+        <v>6.79</v>
+      </c>
+      <c r="E35">
+        <v>5.64</v>
+      </c>
+      <c r="F35">
+        <v>6.15</v>
+      </c>
+      <c r="G35">
+        <v>4.63</v>
+      </c>
+      <c r="H35">
+        <v>5.12</v>
+      </c>
+      <c r="I35">
+        <v>4.12</v>
+      </c>
+      <c r="J35">
+        <v>4.57</v>
+      </c>
+      <c r="K35">
+        <v>4.78</v>
+      </c>
+      <c r="L35">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="M35">
+        <v>5.09</v>
+      </c>
+      <c r="N35">
+        <v>5.35</v>
+      </c>
+      <c r="O35">
+        <v>6.45</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="0"/>
+        <v>5.2750000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="C36">
+        <v>-5.25</v>
+      </c>
+      <c r="D36">
+        <v>6.37</v>
+      </c>
+      <c r="E36">
+        <v>5.52</v>
+      </c>
+      <c r="F36">
+        <v>6.09</v>
+      </c>
+      <c r="G36">
+        <v>4.91</v>
+      </c>
+      <c r="H36">
+        <v>5.34</v>
+      </c>
+      <c r="I36">
+        <v>4.34</v>
+      </c>
+      <c r="J36">
+        <v>4.88</v>
+      </c>
+      <c r="K36">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="L36">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="M36">
+        <v>5.2</v>
+      </c>
+      <c r="N36">
+        <v>6.01</v>
+      </c>
+      <c r="O36">
+        <v>5.99</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="0"/>
+        <v>5.3358333333333334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="C37">
+        <v>-6.2999000000000001</v>
+      </c>
+      <c r="D37">
+        <v>9.11</v>
+      </c>
+      <c r="E37">
+        <v>7.37</v>
+      </c>
+      <c r="F37">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="G37">
+        <v>6.65</v>
+      </c>
+      <c r="H37">
+        <v>6.66</v>
+      </c>
+      <c r="I37">
+        <v>5.74</v>
+      </c>
+      <c r="J37">
+        <v>6.55</v>
+      </c>
+      <c r="K37">
+        <v>6.33</v>
+      </c>
+      <c r="L37">
+        <v>6.34</v>
+      </c>
+      <c r="M37">
+        <v>7.22</v>
+      </c>
+      <c r="N37">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="O37">
+        <v>8.59</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="0"/>
+        <v>7.2891666666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>49.716700000000003</v>
+      </c>
+      <c r="C38">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D38">
+        <v>7.49</v>
+      </c>
+      <c r="E38">
+        <v>6.66</v>
+      </c>
+      <c r="F38">
+        <v>6.88</v>
+      </c>
+      <c r="G38">
+        <v>5.34</v>
+      </c>
+      <c r="H38">
+        <v>5.93</v>
+      </c>
+      <c r="I38">
+        <v>4.83</v>
+      </c>
+      <c r="J38">
+        <v>5.21</v>
+      </c>
+      <c r="K38">
+        <v>5.36</v>
+      </c>
+      <c r="L38">
+        <v>5.6</v>
+      </c>
+      <c r="M38">
+        <v>6.29</v>
+      </c>
+      <c r="N38">
+        <v>7.7</v>
+      </c>
+      <c r="O38">
+        <v>7.37</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="0"/>
+        <v>6.2216666666666667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <v>49.433300000000003</v>
+      </c>
+      <c r="C39">
+        <v>-2.6</v>
+      </c>
+      <c r="D39">
+        <v>6.88</v>
+      </c>
+      <c r="E39">
+        <v>6.2</v>
+      </c>
+      <c r="F39">
+        <v>6.59</v>
+      </c>
+      <c r="G39">
+        <v>5.17</v>
+      </c>
+      <c r="H39">
+        <v>5.69</v>
+      </c>
+      <c r="I39">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="J39">
+        <v>5.36</v>
+      </c>
+      <c r="K39">
+        <v>5.36</v>
+      </c>
+      <c r="L39">
+        <v>5.19</v>
+      </c>
+      <c r="M39">
+        <v>5.59</v>
+      </c>
+      <c r="N39">
+        <v>6.96</v>
+      </c>
+      <c r="O39">
+        <v>6.64</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="0"/>
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>51.4833</v>
+      </c>
+      <c r="C40">
+        <v>-0.45</v>
+      </c>
+      <c r="D40">
+        <v>5.49</v>
+      </c>
+      <c r="E40">
+        <v>3.97</v>
+      </c>
+      <c r="F40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G40">
+        <v>3.76</v>
+      </c>
+      <c r="H40">
+        <v>4.28</v>
+      </c>
+      <c r="I40">
+        <v>3.87</v>
+      </c>
+      <c r="J40">
+        <v>4.24</v>
+      </c>
+      <c r="K40">
+        <v>3.73</v>
+      </c>
+      <c r="L40">
+        <v>3.65</v>
+      </c>
+      <c r="M40">
+        <v>3.63</v>
+      </c>
+      <c r="N40">
+        <v>3.97</v>
+      </c>
+      <c r="O40">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="0"/>
+        <v>4.1158333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>51.616700000000002</v>
+      </c>
+      <c r="C41">
+        <v>-1.0832999999999999</v>
+      </c>
+      <c r="D41">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E41">
+        <v>3.81</v>
+      </c>
+      <c r="F41">
+        <v>4.55</v>
+      </c>
+      <c r="G41">
+        <v>3.79</v>
+      </c>
+      <c r="H41">
+        <v>4.01</v>
+      </c>
+      <c r="I41">
+        <v>3.28</v>
+      </c>
+      <c r="J41">
+        <v>3.94</v>
+      </c>
+      <c r="K41">
+        <v>3.68</v>
+      </c>
+      <c r="L41">
+        <v>3.62</v>
+      </c>
+      <c r="M41">
+        <v>3.77</v>
+      </c>
+      <c r="N41">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="O41">
+        <v>3.76</v>
+      </c>
+      <c r="P41">
+        <f>AVERAGE(E41:O41)</f>
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>51.5</v>
+      </c>
+      <c r="C42">
+        <v>-1.9832000000000001</v>
+      </c>
+      <c r="D42">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E42">
+        <v>4.54</v>
+      </c>
+      <c r="F42">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="G42">
+        <v>4.33</v>
+      </c>
+      <c r="H42">
+        <v>4.59</v>
+      </c>
+      <c r="I42">
+        <v>3.82</v>
+      </c>
+      <c r="J42">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="K42">
+        <v>4.03</v>
+      </c>
+      <c r="L42">
+        <v>3.99</v>
+      </c>
+      <c r="M42">
+        <v>4.18</v>
+      </c>
+      <c r="N42">
+        <v>4.63</v>
+      </c>
+      <c r="O42">
+        <v>4.37</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="0"/>
+        <v>4.4041666666666677</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43">
+        <v>51.5167</v>
+      </c>
+      <c r="C43">
+        <v>-2.5832999999999999</v>
+      </c>
+      <c r="D43">
+        <v>5.31</v>
+      </c>
+      <c r="E43">
+        <v>4.51</v>
+      </c>
+      <c r="F43">
+        <v>5.29</v>
+      </c>
+      <c r="G43">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="H43">
+        <v>5.04</v>
+      </c>
+      <c r="I43">
+        <v>4.42</v>
+      </c>
+      <c r="J43">
+        <v>5.12</v>
+      </c>
+      <c r="K43">
+        <v>4.87</v>
+      </c>
+      <c r="L43">
+        <v>4.62</v>
+      </c>
+      <c r="M43">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="N43">
+        <v>4.96</v>
+      </c>
+      <c r="O43">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>4.7816666666666654</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44">
+        <v>51.383299999999998</v>
+      </c>
+      <c r="C44">
+        <v>-2.7166899999999998</v>
+      </c>
+      <c r="D44">
+        <v>5.74</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>5.6</v>
+      </c>
+      <c r="G44">
+        <v>4.78</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>4.17</v>
+      </c>
+      <c r="J44">
+        <v>4.74</v>
+      </c>
+      <c r="K44">
+        <v>4.5</v>
+      </c>
+      <c r="L44">
+        <v>4.42</v>
+      </c>
+      <c r="M44">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N44">
+        <v>5.2</v>
+      </c>
+      <c r="O44">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="0"/>
+        <v>4.8866666666666676</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45">
+        <v>51</v>
+      </c>
+      <c r="C45">
+        <v>-2.6332900000000001</v>
+      </c>
+      <c r="D45">
+        <v>4.34</v>
+      </c>
+      <c r="E45">
+        <v>3.71</v>
+      </c>
+      <c r="F45">
+        <v>4.59</v>
+      </c>
+      <c r="G45">
+        <v>3.51</v>
+      </c>
+      <c r="H45">
+        <v>3.79</v>
+      </c>
+      <c r="I45">
+        <v>3.16</v>
+      </c>
+      <c r="J45">
+        <v>3.88</v>
+      </c>
+      <c r="K45">
+        <v>3.67</v>
+      </c>
+      <c r="L45">
+        <v>3.25</v>
+      </c>
+      <c r="M45">
+        <v>3.44</v>
+      </c>
+      <c r="N45">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="O45">
+        <v>3.56</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="0"/>
+        <v>3.7433333333333336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46">
+        <v>50.783299999999997</v>
+      </c>
+      <c r="C46">
+        <v>-1.833</v>
+      </c>
+      <c r="D46">
+        <v>4.88</v>
+      </c>
+      <c r="E46">
+        <v>4.2</v>
+      </c>
+      <c r="F46">
+        <v>4.83</v>
+      </c>
+      <c r="G46">
+        <v>4.09</v>
+      </c>
+      <c r="H46">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="I46">
+        <v>3.88</v>
+      </c>
+      <c r="J46">
+        <v>4.41</v>
+      </c>
+      <c r="K46">
+        <v>4.25</v>
+      </c>
+      <c r="L46">
+        <v>3.9</v>
+      </c>
+      <c r="M46">
+        <v>3.91</v>
+      </c>
+      <c r="N46">
+        <v>4.49</v>
+      </c>
+      <c r="O46">
+        <v>4.01</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="0"/>
+        <v>4.2774999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47">
+        <v>51.15</v>
+      </c>
+      <c r="C47">
+        <v>-0.18329999999999999</v>
+      </c>
+      <c r="D47">
+        <v>3.93</v>
+      </c>
+      <c r="E47">
+        <v>3.46</v>
+      </c>
+      <c r="F47">
+        <v>3.95</v>
+      </c>
+      <c r="G47">
+        <v>3.21</v>
+      </c>
+      <c r="H47">
+        <v>3.61</v>
+      </c>
+      <c r="I47">
+        <v>3.1</v>
+      </c>
+      <c r="J47">
+        <v>3.43</v>
+      </c>
+      <c r="K47">
+        <v>3.24</v>
+      </c>
+      <c r="L47">
+        <v>2.99</v>
+      </c>
+      <c r="M47">
+        <v>2.93</v>
+      </c>
+      <c r="N47">
+        <v>3.54</v>
+      </c>
+      <c r="O47">
+        <v>3.33</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="0"/>
+        <v>3.3933333333333331</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48">
+        <v>51.75</v>
+      </c>
+      <c r="C48">
+        <v>-1.5832999999999999</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>3.67</v>
+      </c>
+      <c r="F48">
+        <v>4.13</v>
+      </c>
+      <c r="G48">
+        <v>3.48</v>
+      </c>
+      <c r="H48">
+        <v>3.69</v>
+      </c>
+      <c r="I48">
+        <v>2.96</v>
+      </c>
+      <c r="J48">
+        <v>3.2</v>
+      </c>
+      <c r="K48">
+        <v>3.19</v>
+      </c>
+      <c r="L48">
+        <v>3.12</v>
+      </c>
+      <c r="M48">
+        <v>3.05</v>
+      </c>
+      <c r="N48">
+        <v>3.52</v>
+      </c>
+      <c r="O48">
+        <v>3.39</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="0"/>
+        <v>3.4500000000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49">
+        <v>51.9</v>
+      </c>
+      <c r="C49">
+        <v>-2.16669</v>
+      </c>
+      <c r="D49">
+        <v>3.82</v>
+      </c>
+      <c r="E49">
+        <v>3.13</v>
+      </c>
+      <c r="F49">
+        <v>4.25</v>
+      </c>
+      <c r="G49">
+        <v>3.58</v>
+      </c>
+      <c r="H49">
+        <v>3.78</v>
+      </c>
+      <c r="I49">
+        <v>3.13</v>
+      </c>
+      <c r="J49">
+        <v>3.81</v>
+      </c>
+      <c r="K49">
+        <v>3.71</v>
+      </c>
+      <c r="L49">
+        <v>3.32</v>
+      </c>
+      <c r="M49">
+        <v>3.21</v>
+      </c>
+      <c r="N49">
+        <v>3.48</v>
+      </c>
+      <c r="O49">
+        <v>2.64</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>3.4883333333333328</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50">
+        <v>52.45</v>
+      </c>
+      <c r="C50">
+        <v>-1.7332989999999999</v>
+      </c>
+      <c r="D50">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="E50">
+        <v>3.94</v>
+      </c>
+      <c r="F50">
+        <v>4.7</v>
+      </c>
+      <c r="G50">
+        <v>3.9</v>
+      </c>
+      <c r="H50">
+        <v>4.05</v>
+      </c>
+      <c r="I50">
+        <v>3.6</v>
+      </c>
+      <c r="J50">
+        <v>4.04</v>
+      </c>
+      <c r="K50">
+        <v>4.04</v>
+      </c>
+      <c r="L50">
+        <v>3.74</v>
+      </c>
+      <c r="M50">
+        <v>3.78</v>
+      </c>
+      <c r="N50">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="O50">
+        <v>3.83</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>4.0516666666666667</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51">
+        <v>52.066699999999997</v>
+      </c>
+      <c r="C51">
+        <v>-0.61670000000000003</v>
+      </c>
+      <c r="D51">
+        <v>5.96</v>
+      </c>
+      <c r="E51">
+        <v>5.16</v>
+      </c>
+      <c r="F51">
+        <v>6.32</v>
+      </c>
+      <c r="G51">
+        <v>5.2</v>
+      </c>
+      <c r="H51">
+        <v>5.49</v>
+      </c>
+      <c r="I51">
+        <v>4.38</v>
+      </c>
+      <c r="J51">
+        <v>5.21</v>
+      </c>
+      <c r="K51">
+        <v>5.34</v>
+      </c>
+      <c r="L51">
+        <v>5.29</v>
+      </c>
+      <c r="M51">
+        <v>4.93</v>
+      </c>
+      <c r="N51">
+        <v>5.4</v>
+      </c>
+      <c r="O51">
+        <v>4.99</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="0"/>
+        <v>5.3058333333333332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52">
+        <v>51.866700000000002</v>
+      </c>
+      <c r="C52">
+        <v>-0.36670000000000003</v>
+      </c>
+      <c r="D52">
+        <v>5.48</v>
+      </c>
+      <c r="E52">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F52">
+        <v>5.37</v>
+      </c>
+      <c r="G52">
+        <v>4.22</v>
+      </c>
+      <c r="H52">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I52">
+        <v>3.8</v>
+      </c>
+      <c r="J52">
+        <v>4.26</v>
+      </c>
+      <c r="K52">
+        <v>4.28</v>
+      </c>
+      <c r="L52">
+        <v>4.07</v>
+      </c>
+      <c r="M52">
+        <v>4</v>
+      </c>
+      <c r="N52">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="O52">
+        <v>4.63</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="0"/>
+        <v>4.5008333333333344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53">
+        <v>51.883299999999998</v>
+      </c>
+      <c r="C53">
+        <v>0.23329900000000001</v>
+      </c>
+      <c r="D53">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="E53">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F53">
+        <v>4.7</v>
+      </c>
+      <c r="G53">
+        <v>3.91</v>
+      </c>
+      <c r="H53">
+        <v>4.28</v>
+      </c>
+      <c r="I53">
+        <v>3.59</v>
+      </c>
+      <c r="J53">
+        <v>4.17</v>
+      </c>
+      <c r="K53">
+        <v>4.04</v>
+      </c>
+      <c r="L53">
+        <v>3.95</v>
+      </c>
+      <c r="M53">
+        <v>4.01</v>
+      </c>
+      <c r="N53">
+        <v>4.53</v>
+      </c>
+      <c r="O53">
+        <v>4.32</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="0"/>
+        <v>4.2116666666666669</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54">
+        <v>56.5</v>
+      </c>
+      <c r="C54">
+        <v>-6.8832990000000001</v>
+      </c>
+      <c r="D54">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="E54">
+        <v>6.74</v>
+      </c>
+      <c r="F54">
+        <v>8.1</v>
+      </c>
+      <c r="G54">
+        <v>6.44</v>
+      </c>
+      <c r="H54">
+        <v>6.02</v>
+      </c>
+      <c r="I54">
+        <v>5.44</v>
+      </c>
+      <c r="J54">
+        <v>5.88</v>
+      </c>
+      <c r="K54">
+        <v>6.07</v>
+      </c>
+      <c r="L54">
+        <v>6.76</v>
+      </c>
+      <c r="M54">
+        <v>7.45</v>
+      </c>
+      <c r="N54">
+        <v>7.9</v>
+      </c>
+      <c r="O54">
+        <v>7.22</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="0"/>
+        <v>6.9074999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="C55">
+        <v>-6.2567000000000004</v>
+      </c>
+      <c r="D55">
+        <v>7.67</v>
+      </c>
+      <c r="E55">
+        <v>5.97</v>
+      </c>
+      <c r="F55">
+        <v>7.09</v>
+      </c>
+      <c r="G55">
+        <v>6.04</v>
+      </c>
+      <c r="H55">
+        <v>5.94</v>
+      </c>
+      <c r="I55">
+        <v>5.09</v>
+      </c>
+      <c r="J55">
+        <v>5.37</v>
+      </c>
+      <c r="K55">
+        <v>5.29</v>
+      </c>
+      <c r="L55">
+        <v>5.9</v>
+      </c>
+      <c r="M55">
+        <v>6.53</v>
+      </c>
+      <c r="N55">
+        <v>6.88</v>
+      </c>
+      <c r="O55">
+        <v>5.48</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="0"/>
+        <v>6.104166666666667</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56">
+        <v>55.433300000000003</v>
+      </c>
+      <c r="C56">
+        <v>-5.6863999999999999</v>
+      </c>
+      <c r="D56">
+        <v>7.47</v>
+      </c>
+      <c r="E56">
+        <v>5.97</v>
+      </c>
+      <c r="F56">
+        <v>7.06</v>
+      </c>
+      <c r="G56">
+        <v>5.94</v>
+      </c>
+      <c r="H56">
+        <v>5.7</v>
+      </c>
+      <c r="I56">
+        <v>4.83</v>
+      </c>
+      <c r="J56">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="K56">
+        <v>5.31</v>
+      </c>
+      <c r="L56">
+        <v>6.07</v>
+      </c>
+      <c r="M56">
+        <v>6.6</v>
+      </c>
+      <c r="N56">
+        <v>7.08</v>
+      </c>
+      <c r="O56">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>55.5</v>
+      </c>
+      <c r="C57">
+        <v>-4.5833000000000004</v>
+      </c>
+      <c r="D57">
+        <v>5.07</v>
+      </c>
+      <c r="E57">
+        <v>3.68</v>
+      </c>
+      <c r="F57">
+        <v>4.62</v>
+      </c>
+      <c r="G57">
+        <v>4.17</v>
+      </c>
+      <c r="H57">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="I57">
+        <v>3.49</v>
+      </c>
+      <c r="J57">
+        <v>3.78</v>
+      </c>
+      <c r="K57">
+        <v>4.09</v>
+      </c>
+      <c r="L57">
+        <v>4.07</v>
+      </c>
+      <c r="M57">
+        <v>4.07</v>
+      </c>
+      <c r="N57">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O57">
+        <v>3.44</v>
       </c>
     </row>
   </sheetData>
@@ -1526,8 +3532,16 @@
     <mergeCell ref="D1:O1"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="P3:P31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="P3:P55">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+      <formula>5.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P17:P55">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>5.7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>5.7</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>